<commit_message>
Made sample names clearer after Georg's email
</commit_message>
<xml_diff>
--- a/docs/Examples/Two_Pyroxene_Thermobarometry/Two_pyroxene_input.xlsx
+++ b/docs/Examples/Two_Pyroxene_Thermobarometry/Two_pyroxene_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Two_pyroxene_Thermobarometry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Two_Pyroxene_Thermobarometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E9C707-3BC5-47C8-9FEE-3077748DD2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A01AEA1-5996-4786-8CFF-BE43C15002CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{273FEE2F-31E7-45B4-9E0B-954A0F6A9368}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="2" xr2:uid="{273FEE2F-31E7-45B4-9E0B-954A0F6A9368}"/>
   </bookViews>
   <sheets>
     <sheet name="Paired_Cpx_Opx" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -176,67 +176,136 @@
     <t>Sample 23</t>
   </si>
   <si>
-    <t>Sample1</t>
-  </si>
-  <si>
-    <t>Sample2</t>
-  </si>
-  <si>
-    <t>Sample3</t>
-  </si>
-  <si>
-    <t>Sample4</t>
-  </si>
-  <si>
-    <t>Sample5</t>
-  </si>
-  <si>
-    <t>Sample6</t>
-  </si>
-  <si>
-    <t>Sample7</t>
-  </si>
-  <si>
-    <t>Sample8</t>
-  </si>
-  <si>
-    <t>Sample9</t>
-  </si>
-  <si>
-    <t>Sample10</t>
-  </si>
-  <si>
-    <t>Sample11</t>
-  </si>
-  <si>
-    <t>Sample12</t>
-  </si>
-  <si>
-    <t>Sample13</t>
-  </si>
-  <si>
-    <t>Sample14</t>
-  </si>
-  <si>
-    <t>Sample15</t>
-  </si>
-  <si>
-    <t>Sample16</t>
-  </si>
-  <si>
-    <t>Sample17</t>
-  </si>
-  <si>
-    <t>Sample18</t>
-  </si>
-  <si>
-    <t>Sample19</t>
-  </si>
-  <si>
     <t>Sample_ID_Opx</t>
   </si>
   <si>
     <t>Sample_ID_Cpx</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_1</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_2</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_3</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_4</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_5</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_6</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_7</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_8</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_9</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_10</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_11</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_12</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_13</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_14</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_15</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_16</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_17</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_18</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_19</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_20</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_21</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_22</t>
+  </si>
+  <si>
+    <t>your_cpx_sample_name_23</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_1</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_2</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_3</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_4</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_5</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_6</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_7</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_8</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_9</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_10</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_11</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_12</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_13</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_14</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_15</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_16</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_17</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_18</t>
+  </si>
+  <si>
+    <t>your_opx_sample_name_19</t>
   </si>
 </sst>
 </file>
@@ -2387,15 +2456,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E19988-CD01-4F46-A7E7-B07123B6E30C}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2430,7 +2502,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4">
         <v>52.3</v>
@@ -2465,7 +2537,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4">
         <v>51.7</v>
@@ -2500,7 +2572,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4">
         <v>51.5</v>
@@ -2535,7 +2607,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4">
         <v>51.06</v>
@@ -2570,7 +2642,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4">
         <v>53.32</v>
@@ -2605,7 +2677,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4">
         <v>51.58</v>
@@ -2640,7 +2712,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4">
         <v>51.12</v>
@@ -2675,7 +2747,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4">
         <v>52.5</v>
@@ -2710,7 +2782,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4">
         <v>51.8</v>
@@ -2745,7 +2817,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4">
         <v>51.67</v>
@@ -2780,7 +2852,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4">
         <v>53</v>
@@ -2815,7 +2887,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4">
         <v>51.64</v>
@@ -2850,7 +2922,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4">
         <v>51.3</v>
@@ -2885,7 +2957,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B15" s="4">
         <v>52.4</v>
@@ -2920,7 +2992,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4">
         <v>52</v>
@@ -2955,7 +3027,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4">
         <v>52.9</v>
@@ -2990,7 +3062,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B18" s="4">
         <v>51.3</v>
@@ -3025,7 +3097,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B19" s="4">
         <v>51.5</v>
@@ -3060,7 +3132,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B20" s="4">
         <v>50.93</v>
@@ -3095,7 +3167,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B21" s="4">
         <v>51.63</v>
@@ -3130,7 +3202,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B22" s="4">
         <v>51.39</v>
@@ -3165,7 +3237,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B23" s="4">
         <v>52.98</v>
@@ -3200,7 +3272,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4">
         <v>53.77</v>
@@ -3234,6 +3306,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3242,15 +3315,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715FBE33-372D-4D70-A95F-EA4F031B91A2}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -3285,7 +3361,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B2" s="5">
         <v>55</v>
@@ -3320,7 +3396,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5">
         <v>52.7</v>
@@ -3355,7 +3431,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5">
         <v>53.2</v>
@@ -3390,7 +3466,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B5" s="5">
         <v>55.15</v>
@@ -3425,7 +3501,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B6" s="5">
         <v>56.32</v>
@@ -3460,7 +3536,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5">
         <v>54.4</v>
@@ -3495,7 +3571,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5">
         <v>54.1</v>
@@ -3530,7 +3606,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5">
         <v>55.2</v>
@@ -3565,7 +3641,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B10" s="5">
         <v>54.1</v>
@@ -3600,7 +3676,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B11" s="5">
         <v>54.2</v>
@@ -3635,7 +3711,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B12" s="5">
         <v>54.5</v>
@@ -3670,7 +3746,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B13" s="5">
         <v>53.3</v>
@@ -3705,7 +3781,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B14" s="5">
         <v>52.9</v>
@@ -3740,7 +3816,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B15" s="5">
         <v>55</v>
@@ -3775,7 +3851,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B16" s="5">
         <v>54</v>
@@ -3810,7 +3886,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="B17" s="5">
         <v>54.9</v>
@@ -3845,7 +3921,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B18" s="5">
         <v>52.3</v>
@@ -3880,7 +3956,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B19" s="5">
         <v>52.6</v>
@@ -3915,7 +3991,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B20" s="5">
         <v>52.95</v>

</xml_diff>